<commit_message>
add listeners for test execution control and logging; implement JSON and CSV data providers
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testData.xlsx
+++ b/src/test/resources/testdata/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RohithKatta\eclipse-workspace\selenium-testng-framework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACA70291-8599-4446-A8F1-22399279F14C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187C06E0-0E9D-4B9C-97DB-BA348334AFA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,10 +33,10 @@
     <t>password</t>
   </si>
   <si>
-    <t>firstname</t>
+    <t>Admin</t>
   </si>
   <si>
-    <t>lastname</t>
+    <t>admin123</t>
   </si>
 </sst>
 </file>
@@ -354,68 +354,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
-      <c r="D2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>6</v>
-      </c>
-      <c r="C3">
-        <v>7</v>
-      </c>
-      <c r="D3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>9</v>
-      </c>
-      <c r="B4">
-        <v>10</v>
-      </c>
-      <c r="C4">
-        <v>11</v>
-      </c>
-      <c r="D4">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: reorganize listener classes and integrate ExtentReports for enhanced reporting
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testData.xlsx
+++ b/src/test/resources/testdata/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RohithKatta\eclipse-workspace\selenium-testng-framework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187C06E0-0E9D-4B9C-97DB-BA348334AFA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D19741F5-D5C6-411F-BE7F-C93D23DB2C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>username</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>admin123</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>ad123</t>
   </si>
 </sst>
 </file>
@@ -354,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -372,9 +378,25 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Extent reports feature (#8)
* refactor: reorganize listener classes and integrate ExtentReports for enhanced reporting

* chore: add Extent-output to .gitignore for cleaner build output
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testData.xlsx
+++ b/src/test/resources/testdata/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RohithKatta\eclipse-workspace\selenium-testng-framework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187C06E0-0E9D-4B9C-97DB-BA348334AFA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D19741F5-D5C6-411F-BE7F-C93D23DB2C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>username</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>admin123</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>ad123</t>
   </si>
 </sst>
 </file>
@@ -354,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -372,9 +378,25 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Integrate retry logic and data provider enhancements; add method interceptor and annotation transformer for test execution control
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testData.xlsx
+++ b/src/test/resources/testdata/testData.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RohithKatta\eclipse-workspace\selenium-testng-framework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D19741F5-D5C6-411F-BE7F-C93D23DB2C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5064222-9DB8-4CC1-80EC-18D8D4F1D139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7785" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TestsRunner" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>username</t>
   </si>
@@ -43,6 +44,33 @@
   </si>
   <si>
     <t>ad123</t>
+  </si>
+  <si>
+    <t>TestCase</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>loginLogoutTest</t>
+  </si>
+  <si>
+    <t>validate OrangeHRM login and logout functionality</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>homePageTitleTest</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>validate title of home page</t>
+  </si>
+  <si>
+    <t>Execute</t>
   </si>
 </sst>
 </file>
@@ -362,7 +390,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -403,4 +431,56 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1063754B-EDB9-44D8-8B50-09C0A204AF09}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="48.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Integrate retry logic and data provider enhancements; add method interceptor and annotation transformer for test execution control (#9)
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testData.xlsx
+++ b/src/test/resources/testdata/testData.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RohithKatta\eclipse-workspace\selenium-testng-framework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D19741F5-D5C6-411F-BE7F-C93D23DB2C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5064222-9DB8-4CC1-80EC-18D8D4F1D139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7785" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TestsRunner" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>username</t>
   </si>
@@ -43,6 +44,33 @@
   </si>
   <si>
     <t>ad123</t>
+  </si>
+  <si>
+    <t>TestCase</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>loginLogoutTest</t>
+  </si>
+  <si>
+    <t>validate OrangeHRM login and logout functionality</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>homePageTitleTest</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>validate title of home page</t>
+  </si>
+  <si>
+    <t>Execute</t>
   </si>
 </sst>
 </file>
@@ -362,7 +390,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -403,4 +431,56 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1063754B-EDB9-44D8-8B50-09C0A204AF09}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="48.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add multi-browser support and custom annotations for test categorization and authorship; implement retry logic for failed tests
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testData.xlsx
+++ b/src/test/resources/testdata/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RohithKatta\eclipse-workspace\selenium-testng-framework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5064222-9DB8-4CC1-80EC-18D8D4F1D139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF35AE01-18F1-447E-A1CC-190BE0C3BC53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7785" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="18">
   <si>
     <t>username</t>
   </si>
@@ -71,6 +71,15 @@
   </si>
   <si>
     <t>Execute</t>
+  </si>
+  <si>
+    <t>Browser</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>firefox</t>
   </si>
 </sst>
 </file>
@@ -391,7 +400,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -435,19 +444,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1063754B-EDB9-44D8-8B50-09C0A204AF09}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="2" width="48.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -455,10 +465,19 @@
         <v>7</v>
       </c>
       <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -466,18 +485,76 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
         <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Multi browser support, custom annotations and dependency injection (#10)
* Add multi-browser support and custom annotations for test categorization and authorship; implement retry logic for failed tests

* Add CategoryType enum and update FrameWorkAnnotation to use CategoryType for test categorization
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testData.xlsx
+++ b/src/test/resources/testdata/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RohithKatta\eclipse-workspace\selenium-testng-framework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5064222-9DB8-4CC1-80EC-18D8D4F1D139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF35AE01-18F1-447E-A1CC-190BE0C3BC53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7785" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="18">
   <si>
     <t>username</t>
   </si>
@@ -71,6 +71,15 @@
   </si>
   <si>
     <t>Execute</t>
+  </si>
+  <si>
+    <t>Browser</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>firefox</t>
   </si>
 </sst>
 </file>
@@ -391,7 +400,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -435,19 +444,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1063754B-EDB9-44D8-8B50-09C0A204AF09}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="2" width="48.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -455,10 +465,19 @@
         <v>7</v>
       </c>
       <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -466,18 +485,76 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
         <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor code documentation and improve class descriptions across the framework
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testData.xlsx
+++ b/src/test/resources/testdata/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RohithKatta\eclipse-workspace\selenium-testng-framework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF35AE01-18F1-447E-A1CC-190BE0C3BC53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B834ED0-7663-4DCE-BC65-BF29DAD9B075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -447,7 +447,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Refactor code documentation and improve class descriptions across the framework (#12)
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testData.xlsx
+++ b/src/test/resources/testdata/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RohithKatta\eclipse-workspace\selenium-testng-framework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF35AE01-18F1-447E-A1CC-190BE0C3BC53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B834ED0-7663-4DCE-BC65-BF29DAD9B075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -447,7 +447,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Integrate Dockerized Selenium Grid for parallel testing across multiple browsers and versions; enhance driver initialization with version support and update configuration properties.
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testData.xlsx
+++ b/src/test/resources/testdata/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RohithKatta\eclipse-workspace\selenium-testng-framework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B834ED0-7663-4DCE-BC65-BF29DAD9B075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA3624C-0198-43C0-A5FC-8739CF113B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7785" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="23">
   <si>
     <t>username</t>
   </si>
@@ -64,9 +64,6 @@
     <t>homePageTitleTest</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>validate title of home page</t>
   </si>
   <si>
@@ -80,13 +77,41 @@
   </si>
   <si>
     <t>firefox</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>edge</t>
+  </si>
+  <si>
+    <t>latest</t>
+  </si>
+  <si>
+    <t>95.0</t>
+  </si>
+  <si>
+    <t>128.0</t>
+  </si>
+  <si>
+    <t>135.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,13 +137,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -444,120 +474,229 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1063754B-EDB9-44D8-8B50-09C0A204AF09}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="48.28515625" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="45.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
-        <v>15</v>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="D1" t="s">
         <v>14</v>
       </c>
       <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
-        <v>16</v>
+      <c r="C2" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>16</v>
+      <c r="C3" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
-        <v>17</v>
+      <c r="C4" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
         <v>10</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>2</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>10</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>2</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refactor driver initialization and configuration management; enhance error handling and improve code readability
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testData.xlsx
+++ b/src/test/resources/testdata/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RohithKatta\eclipse-workspace\selenium-testng-framework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA3624C-0198-43C0-A5FC-8739CF113B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2B3B90F-2B08-4063-B016-41317AA795AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7785" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -477,7 +477,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Refactor driver initialization and configuration management; enhance error handling and improve code readability (#14)
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testData.xlsx
+++ b/src/test/resources/testdata/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RohithKatta\eclipse-workspace\selenium-testng-framework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA3624C-0198-43C0-A5FC-8739CF113B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2B3B90F-2B08-4063-B016-41317AA795AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7785" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -477,7 +477,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>